<commit_message>
added shortestServiceFirst or firstInFirstOut choice
</commit_message>
<xml_diff>
--- a/DES/Results.xlsx
+++ b/DES/Results.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\StoSim\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59725D42-BB98-4F65-A842-2572030A9472}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" activeTab="1" xr2:uid="{DF063E33-3D5D-45C4-8C12-5D001D08946A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="239000" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -32,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>n</t>
   </si>
@@ -79,53 +76,57 @@
     <t>lambda = 4</t>
   </si>
   <si>
-    <t>mm 0.12644373922774288
-sm 0.02340474318106437
-ms 0.21784042773148599
-ss 0.04523801951111897</t>
-  </si>
-  <si>
-    <t>mm 0.04247853592802712
-sm 0.009525372257121443
-ms 0.0922917608498226
-ss 0.01994193606088075</t>
-  </si>
-  <si>
-    <t>mm 0.017923994616841007
-sm 0.0029966024954689763
-ms 0.06863753483262937
-ss 0.010918541524754213</t>
-  </si>
-  <si>
-    <t>mm 0.0019640834920377236
-sm 0.0008290056502335933
-ms 0.01584730926836269
-ss 0.005766575037450752</t>
-  </si>
-  <si>
-    <t>mm 6.401318809616185e-05
-sm 0.00010217420081242451
-ms 0.0013851004382435966
-ss 0.0018675332497654416</t>
-  </si>
-  <si>
-    <t>mm 1.951369629932742e-07
-sm 2.742840515769929e-06
-ms 6.167686429441128e-06
-ss 8.669285392034401e-05</t>
-  </si>
-  <si>
-    <t>mu = 8</t>
+    <t xml:space="preserve">mu = </t>
+  </si>
+  <si>
+    <t>('mm', 2.8412210131604034)</t>
+  </si>
+  <si>
+    <t>('sm', 0.9811644116700584)</t>
+  </si>
+  <si>
+    <t>('ms', 2.175353282362092)</t>
+  </si>
+  <si>
+    <t>('ss', 0.5750325804528916)</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>sm</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>ss</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,16 +149,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -216,7 +222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -268,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -462,29 +468,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69DE56CA-3E84-464E-BBEE-CCA323686AB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="28.5" customWidth="1"/>
+    <col min="5" max="5" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="69.5" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -515,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="61.75" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
@@ -526,99 +532,441 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D134E7A-AC90-4709-9A9B-44091C55122A}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" customWidth="1"/>
-    <col min="4" max="4" width="28.44140625" customWidth="1"/>
-    <col min="5" max="5" width="26.88671875" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="61.75" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="1"/>
+      <c r="H2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="61.75" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="64.75" customHeight="1">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="H4">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="66.5" customHeight="1">
       <c r="A5">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="H5">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
         <v>15</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.8412210131603999</v>
+      </c>
+      <c r="D12">
+        <v>1.4455454680583599</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0.98116441167005797</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0.47861987539468798</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>2.17535328236209</v>
+      </c>
+      <c r="D14">
+        <v>1.19274691069803</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="G14">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15">
+        <v>0.57503258045289096</v>
+      </c>
+      <c r="D15">
+        <v>0.30191922206865202</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0.176723016118394</v>
+      </c>
+      <c r="D16">
+        <v>1.4008901851842299</v>
+      </c>
+      <c r="G16">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>3.2235592498966202E-2</v>
+      </c>
+      <c r="D17">
+        <v>0.54101142537634095</v>
+      </c>
+      <c r="G17">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>0.40747761939094201</v>
+      </c>
+      <c r="D18">
+        <v>1.1505447807725999</v>
+      </c>
+      <c r="G18">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>6.0207124990259799E-2</v>
+      </c>
+      <c r="D19">
+        <v>0.32238985302463202</v>
+      </c>
+      <c r="G19">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>4.2898171411680803E-3</v>
+      </c>
+      <c r="E20">
+        <v>0.69350736004495905</v>
+      </c>
+      <c r="G20">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>2.4331812811657799E-3</v>
+      </c>
+      <c r="E21">
+        <v>0.29134814838039602</v>
+      </c>
+      <c r="G21">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22">
+        <v>4.3576352947152598E-2</v>
+      </c>
+      <c r="E22">
+        <v>0.606438368441378</v>
+      </c>
+      <c r="G22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>1.9972151355858399E-2</v>
+      </c>
+      <c r="E23">
+        <v>0.14948377542709901</v>
+      </c>
+      <c r="G23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2.73796393958036E-7</v>
+      </c>
+      <c r="D24">
+        <v>1.00401107600786E-4</v>
+      </c>
+      <c r="E24">
+        <v>5.6113094138744704E-3</v>
+      </c>
+      <c r="F24">
+        <v>0.33938527911771599</v>
+      </c>
+      <c r="G24">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.8623734417506103E-6</v>
+      </c>
+      <c r="D25">
+        <v>2.4456991363329303E-4</v>
+      </c>
+      <c r="E25">
+        <v>3.6289818545683201E-3</v>
+      </c>
+      <c r="F25">
+        <v>0.16072450210519701</v>
+      </c>
+      <c r="G25">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="2">
+        <v>8.6538720165646105E-6</v>
+      </c>
+      <c r="D26">
+        <v>2.1787038521057299E-3</v>
+      </c>
+      <c r="E26">
+        <v>3.8208570972822702E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.33288301866108</v>
+      </c>
+      <c r="G26">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>1.2207788773949501E-4</v>
+      </c>
+      <c r="D27">
+        <v>4.68566907259988E-3</v>
+      </c>
+      <c r="E27">
+        <v>1.7312639790972102E-2</v>
+      </c>
+      <c r="F27">
+        <v>9.4192517897446801E-2</v>
+      </c>
+      <c r="G27">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changed plot font size
</commit_message>
<xml_diff>
--- a/DES/Results.xlsx
+++ b/DES/Results.xlsx
@@ -125,7 +125,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +156,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +180,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="133">
+  <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -308,8 +314,134 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -320,8 +452,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="133">
+  <cellStyles count="259">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -388,6 +525,69 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -454,6 +654,69 @@
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -758,7 +1021,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -845,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:AB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20:AC37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -900,7 +1163,7 @@
       <c r="C3" s="1">
         <v>2.8412210131603999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="6">
         <v>1.4455454680583599</v>
       </c>
       <c r="E3" s="1"/>
@@ -919,7 +1182,7 @@
       <c r="C4" s="1">
         <v>0.98116441167005797</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="8">
         <v>0.47861987539468798</v>
       </c>
       <c r="F4" s="1"/>
@@ -937,7 +1200,7 @@
       <c r="C5">
         <v>2.17535328236209</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="6">
         <v>1.19274691069803</v>
       </c>
       <c r="E5" s="1"/>
@@ -955,7 +1218,7 @@
       <c r="C6">
         <v>0.57503258045289096</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>0.30191922206865202</v>
       </c>
       <c r="F6" s="1"/>
@@ -970,7 +1233,7 @@
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>0.176723016118394</v>
       </c>
       <c r="D7">
@@ -987,7 +1250,7 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>3.2235592498966202E-2</v>
       </c>
       <c r="D8">
@@ -1004,7 +1267,7 @@
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>0.40747761939094201</v>
       </c>
       <c r="D9">
@@ -1021,7 +1284,7 @@
       <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>6.0207124990259799E-2</v>
       </c>
       <c r="D10">
@@ -1038,7 +1301,7 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="6">
         <v>4.2898171411680803E-3</v>
       </c>
       <c r="E11">
@@ -1055,7 +1318,7 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="6">
         <v>2.4331812811657799E-3</v>
       </c>
       <c r="E12">
@@ -1072,7 +1335,7 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="6">
         <v>4.3576352947152598E-2</v>
       </c>
       <c r="E13">
@@ -1089,7 +1352,7 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>1.9972151355858399E-2</v>
       </c>
       <c r="E14">
@@ -1106,13 +1369,13 @@
       <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="7">
         <v>2.73796393958036E-7</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="6">
         <v>1.00401107600786E-4</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="6">
         <v>5.6113094138744704E-3</v>
       </c>
       <c r="F15">
@@ -1129,13 +1392,13 @@
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="7">
         <v>3.8623734417506103E-6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="6">
         <v>2.4456991363329303E-4</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="6">
         <v>3.6289818545683201E-3</v>
       </c>
       <c r="F16">
@@ -1145,20 +1408,20 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:28">
       <c r="A17">
         <v>8</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="7">
         <v>8.6538720165646105E-6</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="6">
         <v>2.1787038521057299E-3</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <v>3.8208570972822702E-2</v>
       </c>
       <c r="F17">
@@ -1168,20 +1431,20 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:28">
       <c r="A18">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>1.2207788773949501E-4</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="6">
         <v>4.68566907259988E-3</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="6">
         <v>1.7312639790972102E-2</v>
       </c>
       <c r="F18">
@@ -1191,7 +1454,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:28">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1199,7 +1462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:28">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:28">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1234,8 +1497,10 @@
       <c r="G22">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+    </row>
+    <row r="23" spans="1:28">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1250,8 +1515,10 @@
       <c r="G23">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
+      <c r="Z23" s="1"/>
+      <c r="AB23" s="1"/>
+    </row>
+    <row r="24" spans="1:28">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1265,8 +1532,9 @@
       <c r="G24">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="25" spans="1:28">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1280,8 +1548,9 @@
       <c r="G25">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="AB25" s="1"/>
+    </row>
+    <row r="26" spans="1:28">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1298,7 +1567,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:28">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1312,7 +1581,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:28">
       <c r="A28">
         <v>2</v>
       </c>
@@ -1326,7 +1595,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:28">
       <c r="A29">
         <v>2</v>
       </c>
@@ -1340,7 +1609,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:28">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1357,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:28">
       <c r="A31">
         <v>4</v>
       </c>
@@ -1371,7 +1640,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:28">
       <c r="A32">
         <v>4</v>
       </c>
@@ -1385,7 +1654,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -1399,7 +1668,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:25">
       <c r="A34">
         <v>8</v>
       </c>
@@ -1416,8 +1685,9 @@
       <c r="I34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:9">
+      <c r="Y34" s="2"/>
+    </row>
+    <row r="35" spans="1:25">
       <c r="A35">
         <v>8</v>
       </c>
@@ -1434,8 +1704,9 @@
       <c r="I35" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:9">
+      <c r="Y35" s="2"/>
+    </row>
+    <row r="36" spans="1:25">
       <c r="A36">
         <v>8</v>
       </c>
@@ -1449,8 +1720,9 @@
       <c r="G36">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:9">
+      <c r="Y36" s="2"/>
+    </row>
+    <row r="37" spans="1:25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -1464,7 +1736,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:25">
       <c r="A39" t="s">
         <v>16</v>
       </c>
@@ -1472,7 +1744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1492,7 +1764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -1508,7 +1780,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:25">
       <c r="A42">
         <v>1</v>
       </c>
@@ -1524,7 +1796,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:25">
       <c r="A43">
         <v>1</v>
       </c>
@@ -1539,7 +1811,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -1554,7 +1826,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -1568,7 +1840,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -1582,7 +1854,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -1596,7 +1868,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:25">
       <c r="A48">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Ran at rho = 0.45
</commit_message>
<xml_diff>
--- a/DES/Results.xlsx
+++ b/DES/Results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="25">
   <si>
     <t>n</t>
   </si>
@@ -180,8 +180,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="259">
+  <cellStyleXfs count="271">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -458,7 +470,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="259">
+  <cellStyles count="271">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -588,6 +600,12 @@
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -717,6 +735,12 @@
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1021,7 +1045,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1108,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB75"/>
+  <dimension ref="A1:AB94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20:AC37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1741,7 +1765,7 @@
         <v>16</v>
       </c>
       <c r="C39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:25">
@@ -1772,12 +1796,12 @@
         <v>11</v>
       </c>
       <c r="C41" s="1">
-        <v>16.2059747108678</v>
+        <v>0.37056533376421902</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="42" spans="1:25">
@@ -1788,12 +1812,12 @@
         <v>12</v>
       </c>
       <c r="C42" s="1">
-        <v>13.0219242321655</v>
+        <v>7.1437399224515002E-2</v>
       </c>
       <c r="D42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="43" spans="1:25">
@@ -1804,11 +1828,11 @@
         <v>13</v>
       </c>
       <c r="C43">
-        <v>10.4076880789996</v>
+        <v>0.67918055132176203</v>
       </c>
       <c r="E43" s="1"/>
       <c r="G43">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="44" spans="1:25">
@@ -1819,11 +1843,11 @@
         <v>14</v>
       </c>
       <c r="C44">
-        <v>5.41078376513682</v>
+        <v>0.134130950227037</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="45" spans="1:25">
@@ -1834,10 +1858,10 @@
         <v>11</v>
       </c>
       <c r="D45">
-        <v>7.9327370181821397</v>
+        <v>0.114233170542706</v>
       </c>
       <c r="G45">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="46" spans="1:25">
@@ -1848,10 +1872,10 @@
         <v>12</v>
       </c>
       <c r="D46">
-        <v>7.3392137583649699</v>
+        <v>2.6901048201692701E-2</v>
       </c>
       <c r="G46">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="47" spans="1:25">
@@ -1862,10 +1886,10 @@
         <v>13</v>
       </c>
       <c r="D47">
-        <v>4.9278479656277598</v>
+        <v>0.27577451173793599</v>
       </c>
       <c r="G47">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="48" spans="1:25">
@@ -1876,10 +1900,10 @@
         <v>14</v>
       </c>
       <c r="D48">
-        <v>2.2985346975536798</v>
+        <v>6.1637425837909501E-2</v>
       </c>
       <c r="G48">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1890,10 +1914,10 @@
         <v>11</v>
       </c>
       <c r="E49">
-        <v>4.0138750023172296</v>
+        <v>2.6377619867628099E-2</v>
       </c>
       <c r="G49">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -1904,10 +1928,10 @@
         <v>12</v>
       </c>
       <c r="E50">
-        <v>3.6205035988981198</v>
+        <v>1.04204289148565E-2</v>
       </c>
       <c r="G50">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -1918,10 +1942,10 @@
         <v>13</v>
       </c>
       <c r="E51">
-        <v>2.5382746923506998</v>
+        <v>9.5589308113855104E-2</v>
       </c>
       <c r="G51">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1932,10 +1956,10 @@
         <v>14</v>
       </c>
       <c r="E52">
-        <v>1.2373628178726801</v>
+        <v>2.99983970450803E-2</v>
       </c>
       <c r="G52">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1947,10 +1971,10 @@
       </c>
       <c r="C53" s="2"/>
       <c r="F53">
-        <v>1.81809190972547</v>
+        <v>3.6828157228642202E-3</v>
       </c>
       <c r="G53">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1962,10 +1986,10 @@
       </c>
       <c r="C54" s="2"/>
       <c r="F54">
-        <v>1.5377692407880099</v>
+        <v>2.3829956682283201E-3</v>
       </c>
       <c r="G54">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1977,10 +2001,10 @@
       </c>
       <c r="C55" s="2"/>
       <c r="F55">
-        <v>1.2455507876509999</v>
+        <v>2.3641473676271101E-2</v>
       </c>
       <c r="G55">
-        <v>0.9</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1991,315 +2015,576 @@
         <v>14</v>
       </c>
       <c r="F56">
+        <v>1.22125631881805E-2</v>
+      </c>
+      <c r="G56">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" t="s">
+        <v>5</v>
+      </c>
+      <c r="G59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1">
+        <v>16.2059747108678</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1">
+        <v>13.0219242321655</v>
+      </c>
+      <c r="D61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62">
+        <v>10.4076880789996</v>
+      </c>
+      <c r="E62" s="1"/>
+      <c r="G62">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>14</v>
+      </c>
+      <c r="C63">
+        <v>5.41078376513682</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64">
+        <v>7.9327370181821397</v>
+      </c>
+      <c r="G64">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65">
+        <v>2</v>
+      </c>
+      <c r="B65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65">
+        <v>7.3392137583649699</v>
+      </c>
+      <c r="G65">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66">
+        <v>2</v>
+      </c>
+      <c r="B66" t="s">
+        <v>13</v>
+      </c>
+      <c r="D66">
+        <v>4.9278479656277598</v>
+      </c>
+      <c r="G66">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67">
+        <v>2.2985346975536798</v>
+      </c>
+      <c r="G67">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68">
+        <v>4</v>
+      </c>
+      <c r="B68" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68">
+        <v>4.0138750023172296</v>
+      </c>
+      <c r="G68">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>4</v>
+      </c>
+      <c r="B69" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69">
+        <v>3.6205035988981198</v>
+      </c>
+      <c r="G69">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70">
+        <v>2.5382746923506998</v>
+      </c>
+      <c r="G70">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>4</v>
+      </c>
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+      <c r="E71">
+        <v>1.2373628178726801</v>
+      </c>
+      <c r="G71">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72">
+        <v>8</v>
+      </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="F72">
+        <v>1.81809190972547</v>
+      </c>
+      <c r="G72">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73">
+        <v>8</v>
+      </c>
+      <c r="B73" t="s">
+        <v>12</v>
+      </c>
+      <c r="C73" s="2"/>
+      <c r="F73">
+        <v>1.5377692407880099</v>
+      </c>
+      <c r="G73">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74">
+        <v>8</v>
+      </c>
+      <c r="B74" t="s">
+        <v>13</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="F74">
+        <v>1.2455507876509999</v>
+      </c>
+      <c r="G74">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75">
+        <v>8</v>
+      </c>
+      <c r="B75" t="s">
+        <v>14</v>
+      </c>
+      <c r="F75">
         <v>0.55026617560472002</v>
       </c>
-      <c r="G56">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" s="3" t="s">
+      <c r="G75">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3" t="s">
+      <c r="B77" s="3"/>
+      <c r="C77" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" s="3" t="s">
+      <c r="D77" s="3"/>
+      <c r="E77" s="3"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="3"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3" t="s">
+      <c r="B78" s="3"/>
+      <c r="C78" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D78" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="F78" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="3">
+    <row r="79" spans="1:7">
+      <c r="A79" s="3">
         <v>1</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B79" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C79" s="4">
         <v>8.0125241248768493</v>
       </c>
-      <c r="D60" s="3"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="3">
+      <c r="D79" s="3"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="3">
         <v>1</v>
       </c>
-      <c r="B61" s="3" t="s">
+      <c r="B80" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="4">
+      <c r="C80" s="4">
         <v>3.9657941849277298</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="3">
+      <c r="D80" s="4"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="3">
         <v>1</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C81" s="3">
         <v>6.9297022415098102</v>
       </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="3">
+      <c r="D81" s="3"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="3">
         <v>1</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C82" s="3">
         <v>3.0046779393660201</v>
       </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="4"/>
-      <c r="G63" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="3">
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="4"/>
+      <c r="G82" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="3">
         <v>2</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3">
+      <c r="C83" s="3"/>
+      <c r="D83" s="3">
         <v>4.0660387971794503</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" s="3">
+      <c r="E83" s="3"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="3">
         <v>2</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3">
+      <c r="C84" s="3"/>
+      <c r="D84" s="3">
         <v>2.6762768676148498</v>
       </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="3">
+      <c r="E84" s="3"/>
+      <c r="F84" s="3"/>
+      <c r="G84" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" s="3">
         <v>2</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3">
+      <c r="C85" s="3"/>
+      <c r="D85" s="3">
         <v>3.5492883190424398</v>
       </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="3">
+      <c r="E85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="3">
         <v>2</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B86" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3">
+      <c r="C86" s="3"/>
+      <c r="D86" s="3">
         <v>1.5848257632350899</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="3">
+      <c r="E86" s="3"/>
+      <c r="F86" s="3"/>
+      <c r="G86" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="3">
         <v>4</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3">
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
+      <c r="E87" s="3">
         <v>1.9014499047122799</v>
       </c>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="3">
+      <c r="F87" s="3"/>
+      <c r="G87" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="3">
         <v>4</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3">
+      <c r="C88" s="3"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="3">
         <v>1.1232806527358401</v>
       </c>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="3">
+      <c r="F88" s="3"/>
+      <c r="G88" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="3">
         <v>4</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B89" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3">
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3">
         <v>1.7355356035344101</v>
       </c>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="3">
+      <c r="F89" s="3"/>
+      <c r="G89" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="3">
         <v>4</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B90" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3">
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3">
         <v>0.71140526951264704</v>
       </c>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="3">
+      <c r="F90" s="3"/>
+      <c r="G90" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" s="3">
         <v>8</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B91" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C72" s="5"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3">
+      <c r="C91" s="5"/>
+      <c r="D91" s="3"/>
+      <c r="E91" s="3"/>
+      <c r="F91" s="3">
         <v>0.85303708057657901</v>
       </c>
-      <c r="G72" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="3">
+      <c r="G91" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" s="3">
         <v>8</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B92" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3">
+      <c r="C92" s="5"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="3"/>
+      <c r="F92" s="3">
         <v>0.68930522163200203</v>
       </c>
-      <c r="G73" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="3">
+      <c r="G92" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" s="3">
         <v>8</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B93" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3">
+      <c r="C93" s="5"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3">
         <v>0.82832068141996396</v>
       </c>
-      <c r="G74" s="3">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="3">
+      <c r="G93" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="3">
         <v>8</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="B94" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3">
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3">
         <v>0.42335199448715399</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G94" s="3">
         <v>0.9</v>
       </c>
     </row>

</xml_diff>